<commit_message>
add invidual investment pars, create utils file for excel logic
</commit_message>
<xml_diff>
--- a/output/agencies.xlsx
+++ b/output/agencies.xlsx
@@ -4,10 +4,11 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Agencies" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Individual Investments" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,324 +425,886 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Agency</t>
+          <t>Department of Agriculture</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Total spending</t>
+          <t>$2.7B</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Department of Agriculture</t>
+          <t>Department of Commerce</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$2.7B</t>
+          <t>$2.8B</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Department of Commerce</t>
+          <t>Department of Defense</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$2.8B</t>
+          <t>$36B</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Department of Defense</t>
+          <t>Department of Health and Human Services</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>$36B</t>
+          <t>$7.0B</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Department of Health and Human Services</t>
+          <t>Department of the Interior</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$7.0B</t>
+          <t>$1.5B</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Department of the Interior</t>
+          <t>Department of Justice</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>$1.5B</t>
+          <t>$3.1B</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Department of Justice</t>
+          <t>Department of Labor</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$3.1B</t>
+          <t>$819M</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Department of Labor</t>
+          <t>Department of State</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>$819M</t>
+          <t>$2.6B</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Department of State</t>
+          <t>Department of the Treasury</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>$2.6B</t>
+          <t>$5.4B</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Department of the Treasury</t>
+          <t>Social Security Administration</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>$5.4B</t>
+          <t>$2.0B</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Social Security Administration</t>
+          <t>Department of Education</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>$2.0B</t>
+          <t>$1.0B</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Department of Education</t>
+          <t>Department of Energy</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>$1.0B</t>
+          <t>$3.1B</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Department of Energy</t>
+          <t>Environmental Protection Agency</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>$3.1B</t>
+          <t>$385M</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Environmental Protection Agency</t>
+          <t>Department of Transportation</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>$385M</t>
+          <t>$3.5B</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Department of Transportation</t>
+          <t>General Services Administration</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>$3.5B</t>
+          <t>$765M</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>General Services Administration</t>
+          <t>Department of Homeland Security</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>$765M</t>
+          <t>$7.4B</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Department of Homeland Security</t>
+          <t>Department of Housing and Urban Development</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>$7.4B</t>
+          <t>$447M</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Department of Housing and Urban Development</t>
+          <t>National Aeronautics and Space Administration</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>$447M</t>
+          <t>$2.2B</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>National Aeronautics and Space Administration</t>
+          <t>Office of Personnel Management</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>$2.2B</t>
+          <t>$125M</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Office of Personnel Management</t>
+          <t>Small Business Administration</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>$125M</t>
+          <t>$129M</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Small Business Administration</t>
+          <t>Department of Veterans Affairs</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>$129M</t>
+          <t>$9.1B</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Department of Veterans Affairs</t>
+          <t>U.S. Agency for International Development</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>$9.1B</t>
+          <t>$256M</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>U.S. Agency for International Development</t>
+          <t>U.S. Army Corps of Engineers</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>$256M</t>
+          <t>$275M</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>U.S. Army Corps of Engineers</t>
+          <t>National Archives and Records Administration</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>$275M</t>
+          <t>$99.9M</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>National Archives and Records Administration</t>
+          <t>National Science Foundation</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>$99.9M</t>
+          <t>$136M</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>National Science Foundation</t>
+          <t>Nuclear Regulatory Commission</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>$136M</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Nuclear Regulatory Commission</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
           <t>$141M</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>393-000000086</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>National Archives and Records Administration</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Agency &amp; Related Services</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>$26.538</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Major IT</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>393-000000087</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>National Archives and Records Administration</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Citizen Services</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>$11.872</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Major IT</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>393-000000088</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>National Archives and Records Administration</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Legislative Presidential &amp; Museum Services</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>$2.830</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Non-major IT</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>393-000000175</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>National Archives and Records Administration</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Mission Support Services</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>$3.914</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Non-major IT</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>393-999990060</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>National Archives and Records Administration</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>E-Rulemaking</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>$0.011</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Funding Transfer</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>393-999990099</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>National Archives and Records Administration</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>FOIA.gov Portal</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>$0.065</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Funding Transfer</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>393-999990160</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>National Archives and Records Administration</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Grants.Gov</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>$0.028</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Funding Transfer</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>393-999991101</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>National Archives and Records Administration</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Administrative Resource Center (ARC)</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>$4.843</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Funding Transfer</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>393-999991204</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>National Archives and Records Administration</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Interior Business Center (IBC)</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>$1.245</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Funding Transfer</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>393-999991218</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>National Archives and Records Administration</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>USAJobs</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>$0.020</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Funding Transfer</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>393-000000081</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>National Archives and Records Administration</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Network</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>$6.693</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Standard IT Infrastructure</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>393-000000082</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>National Archives and Records Administration</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Data Center and Cloud</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>$1.887</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Standard IT Infrastructure</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>393-000000083</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>National Archives and Records Administration</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>End User</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>$17.240</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Standard IT Infrastructure</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>393-000000250</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>National Archives and Records Administration</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>IT Security and Compliance</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>$7.979</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Standard IT Infrastructure</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>393-000000300</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>National Archives and Records Administration</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>IT Management</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>$14.735</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Standard IT Infrastructure</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>

</xml_diff>